<commit_message>
Fixed Flawless Mechanic, corrected Saturate values and added food
</commit_message>
<xml_diff>
--- a/Level Spreadsheet.xlsx
+++ b/Level Spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nutri Mayhem\NutriCrush-Unity-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF348BA-2493-4816-94BA-6D1C6E2EC8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77592876-3705-48D9-B399-13706FA0D2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A710659-CD1A-4DA5-825F-E0BBB8540E3C}"/>
   </bookViews>
@@ -242,10 +242,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,7 +584,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +636,7 @@
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -649,7 +649,7 @@
         <v>31</v>
       </c>
       <c r="F2">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="G2">
         <v>0.11</v>
@@ -674,7 +674,7 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>45</v>
       </c>
@@ -685,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>0.37</v>
@@ -710,7 +710,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -721,7 +721,7 @@
         <v>30</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5.3</v>
       </c>
       <c r="G4">
         <v>0.37</v>
@@ -746,7 +746,7 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
@@ -759,7 +759,7 @@
         <v>34</v>
       </c>
       <c r="F5">
-        <v>3.4</v>
+        <v>6.67</v>
       </c>
       <c r="G5">
         <v>0.8</v>
@@ -784,7 +784,7 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -795,7 +795,7 @@
         <v>37</v>
       </c>
       <c r="F6">
-        <v>3.7</v>
+        <v>7.33</v>
       </c>
       <c r="G6">
         <v>0.8</v>
@@ -820,7 +820,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B7" s="2"/>
+      <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -831,7 +831,7 @@
         <v>39</v>
       </c>
       <c r="F7">
-        <v>3.9</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>0.8</v>
@@ -856,7 +856,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
@@ -869,7 +869,7 @@
         <v>39</v>
       </c>
       <c r="F8">
-        <v>3.9</v>
+        <v>9.33</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -894,7 +894,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B9" s="2"/>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -905,7 +905,7 @@
         <v>45</v>
       </c>
       <c r="F9">
-        <v>4.5</v>
+        <v>10.67</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -930,7 +930,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -941,7 +941,7 @@
         <v>53</v>
       </c>
       <c r="F10">
-        <v>5.3</v>
+        <v>12.67</v>
       </c>
       <c r="G10">
         <v>1.2</v>
@@ -966,7 +966,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
@@ -979,7 +979,7 @@
         <v>74</v>
       </c>
       <c r="F11">
-        <v>7.4</v>
+        <v>17.329999999999998</v>
       </c>
       <c r="G11">
         <v>1.2</v>
@@ -1004,7 +1004,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>18</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>84</v>
       </c>
       <c r="F12">
-        <v>8.4</v>
+        <v>20</v>
       </c>
       <c r="G12">
         <v>1.5</v>
@@ -1040,7 +1040,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
+      <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>88</v>
       </c>
       <c r="F13">
-        <v>8.8000000000000007</v>
+        <v>21.33</v>
       </c>
       <c r="G13">
         <v>1.5</v>
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
@@ -1089,7 +1089,7 @@
         <v>66</v>
       </c>
       <c r="F14">
-        <v>6.6</v>
+        <v>20</v>
       </c>
       <c r="G14">
         <v>1.5</v>
@@ -1114,7 +1114,7 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>65</v>
       </c>
       <c r="F15">
-        <v>6.5</v>
+        <v>19.329999999999998</v>
       </c>
       <c r="G15">
         <v>1.5</v>
@@ -1150,7 +1150,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
+      <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>19</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>65</v>
       </c>
       <c r="F16">
-        <v>6.5</v>
+        <v>19.329999999999998</v>
       </c>
       <c r="G16">
         <v>1.5</v>
@@ -1186,7 +1186,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
@@ -1199,7 +1199,7 @@
         <v>64</v>
       </c>
       <c r="F17">
-        <v>6.4</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="G17">
         <v>1.5</v>
@@ -1224,7 +1224,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>23</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>63</v>
       </c>
       <c r="F18">
-        <v>6.3</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="G18">
         <v>1.5</v>
@@ -1260,7 +1260,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
+      <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>24</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>62</v>
       </c>
       <c r="F19">
-        <v>6.2</v>
+        <v>18</v>
       </c>
       <c r="G19">
         <v>1.5</v>
@@ -1296,7 +1296,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
@@ -1309,7 +1309,7 @@
         <v>61</v>
       </c>
       <c r="F20">
-        <v>6.1</v>
+        <v>18</v>
       </c>
       <c r="G20">
         <v>1.5</v>
@@ -1334,7 +1334,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B21" s="3"/>
+      <c r="B21" s="2"/>
       <c r="C21" t="s">
         <v>27</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>59</v>
       </c>
       <c r="F21">
-        <v>5.9</v>
+        <v>17.329999999999998</v>
       </c>
       <c r="G21">
         <v>1.5</v>
@@ -1370,7 +1370,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B22" s="3"/>
+      <c r="B22" s="2"/>
       <c r="C22" t="s">
         <v>28</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>56</v>
       </c>
       <c r="F22">
-        <v>5.6</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="G22">
         <v>1.5</v>
@@ -1406,7 +1406,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C23" t="s">
@@ -1419,7 +1419,7 @@
         <v>55</v>
       </c>
       <c r="F23">
-        <v>5.5</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="G23">
         <v>1.5</v>
@@ -1444,7 +1444,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>31</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>54</v>
       </c>
       <c r="F24">
-        <v>5.4</v>
+        <v>16</v>
       </c>
       <c r="G24">
         <v>1.5</v>
@@ -1480,7 +1480,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="2"/>
+      <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>32</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>53</v>
       </c>
       <c r="F25">
-        <v>5.3</v>
+        <v>15.33</v>
       </c>
       <c r="G25">
         <v>1.5</v>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" t="s">
@@ -1529,7 +1529,7 @@
         <v>52</v>
       </c>
       <c r="F26">
-        <v>5.2</v>
+        <v>15.33</v>
       </c>
       <c r="G26">
         <v>1.5</v>
@@ -1554,7 +1554,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B27" s="2"/>
+      <c r="B27" s="3"/>
       <c r="C27" t="s">
         <v>37</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>51</v>
       </c>
       <c r="F27">
-        <v>5.0999999999999996</v>
+        <v>14.67</v>
       </c>
       <c r="G27">
         <v>1.5</v>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B28" s="2"/>
+      <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>35</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>50</v>
       </c>
       <c r="F28">
-        <v>5</v>
+        <v>14.67</v>
       </c>
       <c r="G28">
         <v>1.5</v>
@@ -1626,7 +1626,7 @@
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C29" t="s">
@@ -1639,7 +1639,7 @@
         <v>49</v>
       </c>
       <c r="F29">
-        <v>4.9000000000000004</v>
+        <v>14</v>
       </c>
       <c r="G29">
         <v>1.5</v>
@@ -1664,7 +1664,7 @@
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
+      <c r="B30" s="3"/>
       <c r="C30" t="s">
         <v>39</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>48</v>
       </c>
       <c r="F30">
-        <v>4.8</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <v>1.5</v>
@@ -1700,7 +1700,7 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
+      <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>40</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>47</v>
       </c>
       <c r="F31">
-        <v>4.7</v>
+        <v>13.33</v>
       </c>
       <c r="G31">
         <v>1.5</v>

</xml_diff>